<commit_message>
Modificaciones en nombres de recursos
Modificaciones en nombres de recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion12/Escaleta_CN_10_12_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion12/Escaleta_CN_10_12_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado10\guion12\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -612,12 +617,6 @@
     <t>Competencias</t>
   </si>
   <si>
-    <t>Competencias: determinación de la composición porcentual</t>
-  </si>
-  <si>
-    <t>Actividad que propone una práctica de laboratorio para conocer la composición porcentual de un compuesto</t>
-  </si>
-  <si>
     <t>Recurso M101AP-01</t>
   </si>
   <si>
@@ -690,9 +689,6 @@
     <t>Recurso M1A-02</t>
   </si>
   <si>
-    <t xml:space="preserve">Animación que muestra el proceso para realizar conversiones de masa, moles y número de partículas </t>
-  </si>
-  <si>
     <t>Recursos adicionales 01</t>
   </si>
   <si>
@@ -715,6 +711,15 @@
   </si>
   <si>
     <t>Actividad que propone realizar una investigación bibliográfica sobre el número Avogadro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secuencia  de imágenes que muestra el proceso para realizar conversiones de masa, moles y número de partículas </t>
+  </si>
+  <si>
+    <t>Competencias: porcentaje de agua en una sal hidratada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad que propone una práctica de laboratorio para determinar el porcentaje de agua en el sulfato cúprico </t>
   </si>
 </sst>
 </file>
@@ -936,77 +941,8 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1020,6 +956,75 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1080,7 +1085,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1115,7 +1120,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1326,125 +1331,125 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K25" sqref="A25:XFD25"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="29" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" style="29" customWidth="1"/>
-    <col min="4" max="4" width="34" style="29" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" style="52" customWidth="1"/>
-    <col min="7" max="7" width="64.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="52" customWidth="1"/>
-    <col min="9" max="9" width="11" style="52" customWidth="1"/>
-    <col min="10" max="10" width="89.7109375" style="29" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" style="29" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" style="29" customWidth="1"/>
-    <col min="13" max="14" width="9.28515625" style="29" customWidth="1"/>
-    <col min="15" max="15" width="17.85546875" style="52" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" style="52" customWidth="1"/>
-    <col min="17" max="17" width="20.42578125" style="52" customWidth="1"/>
-    <col min="18" max="18" width="23" style="29" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="27.85546875" style="29" customWidth="1"/>
-    <col min="20" max="20" width="25.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.7109375" style="29" customWidth="1"/>
-    <col min="22" max="16384" width="11.42578125" style="29"/>
+    <col min="1" max="1" width="16.5703125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" style="17" customWidth="1"/>
+    <col min="4" max="4" width="34" style="17" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" style="29" customWidth="1"/>
+    <col min="7" max="7" width="64.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="29" customWidth="1"/>
+    <col min="9" max="9" width="11" style="29" customWidth="1"/>
+    <col min="10" max="10" width="89.7109375" style="17" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="17" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="17" customWidth="1"/>
+    <col min="13" max="14" width="9.28515625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" style="29" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" style="29" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" style="29" customWidth="1"/>
+    <col min="18" max="18" width="23" style="17" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.85546875" style="17" customWidth="1"/>
+    <col min="20" max="20" width="25.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.7109375" style="17" customWidth="1"/>
+    <col min="22" max="16384" width="11.42578125" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="24"/>
-      <c r="O1" s="25" t="s">
+      <c r="N1" s="50"/>
+      <c r="O1" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="P1" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="26" t="s">
+      <c r="Q1" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="27" t="s">
+      <c r="R1" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="26" t="s">
+      <c r="S1" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="28" t="s">
+      <c r="T1" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="26" t="s">
+      <c r="U1" s="32" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="37" t="s">
+      <c r="A2" s="43"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="N2" s="37" t="s">
+      <c r="N2" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="41"/>
-      <c r="U2" s="39"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="33"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -1456,12 +1461,12 @@
       <c r="C3" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="19" t="s">
         <v>124</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="11"/>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="20" t="s">
         <v>150</v>
       </c>
       <c r="H3" s="11">
@@ -1470,8 +1475,8 @@
       <c r="I3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="44" t="s">
-        <v>209</v>
+      <c r="J3" s="21" t="s">
+        <v>207</v>
       </c>
       <c r="K3" s="13" t="s">
         <v>20</v>
@@ -1483,23 +1488,23 @@
         <v>54</v>
       </c>
       <c r="N3" s="14"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45" t="s">
+      <c r="O3" s="22"/>
+      <c r="P3" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="46">
+      <c r="Q3" s="23">
         <v>6</v>
       </c>
-      <c r="R3" s="47" t="s">
+      <c r="R3" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="S3" s="46" t="s">
+      <c r="S3" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="T3" s="48" t="s">
+      <c r="T3" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="U3" s="46" t="s">
+      <c r="U3" s="23" t="s">
         <v>154</v>
       </c>
     </row>
@@ -1513,13 +1518,13 @@
       <c r="C4" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="19" t="s">
         <v>124</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="11"/>
-      <c r="G4" s="43" t="s">
-        <v>212</v>
+      <c r="G4" s="20" t="s">
+        <v>210</v>
       </c>
       <c r="H4" s="11">
         <v>2</v>
@@ -1527,7 +1532,7 @@
       <c r="I4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="44" t="s">
+      <c r="J4" s="21" t="s">
         <v>165</v>
       </c>
       <c r="K4" s="13" t="s">
@@ -1540,23 +1545,23 @@
       <c r="N4" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45" t="s">
+      <c r="O4" s="22"/>
+      <c r="P4" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="46">
+      <c r="Q4" s="23">
         <v>6</v>
       </c>
-      <c r="R4" s="47" t="s">
+      <c r="R4" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S4" s="46" t="s">
+      <c r="S4" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T4" s="48" t="s">
+      <c r="T4" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="U4" s="46" t="s">
+      <c r="U4" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1570,12 +1575,12 @@
       <c r="C5" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="19" t="s">
         <v>124</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="11"/>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="20" t="s">
         <v>167</v>
       </c>
       <c r="H5" s="11">
@@ -1584,7 +1589,7 @@
       <c r="I5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="44" t="s">
+      <c r="J5" s="21" t="s">
         <v>170</v>
       </c>
       <c r="K5" s="13" t="s">
@@ -1597,23 +1602,23 @@
       <c r="N5" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45" t="s">
+      <c r="O5" s="22"/>
+      <c r="P5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="46">
+      <c r="Q5" s="23">
         <v>6</v>
       </c>
-      <c r="R5" s="47" t="s">
+      <c r="R5" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S5" s="46" t="s">
+      <c r="S5" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T5" s="48" t="s">
+      <c r="T5" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="U5" s="46" t="s">
+      <c r="U5" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1627,13 +1632,13 @@
       <c r="C6" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="19" t="s">
         <v>124</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="11"/>
-      <c r="G6" s="43" t="s">
-        <v>210</v>
+      <c r="G6" s="20" t="s">
+        <v>208</v>
       </c>
       <c r="H6" s="11">
         <v>4</v>
@@ -1641,7 +1646,7 @@
       <c r="I6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="44" t="s">
+      <c r="J6" s="21" t="s">
         <v>169</v>
       </c>
       <c r="K6" s="13" t="s">
@@ -1654,23 +1659,23 @@
       <c r="N6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="O6" s="45"/>
-      <c r="P6" s="45" t="s">
+      <c r="O6" s="22"/>
+      <c r="P6" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" s="46">
+      <c r="Q6" s="23">
         <v>6</v>
       </c>
-      <c r="R6" s="47" t="s">
+      <c r="R6" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S6" s="46" t="s">
+      <c r="S6" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T6" s="48" t="s">
+      <c r="T6" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="U6" s="46" t="s">
+      <c r="U6" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1684,14 +1689,14 @@
       <c r="C7" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="E7" s="49" t="s">
+      <c r="E7" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="F7" s="50"/>
-      <c r="G7" s="43" t="s">
+      <c r="F7" s="27"/>
+      <c r="G7" s="20" t="s">
         <v>134</v>
       </c>
       <c r="H7" s="11">
@@ -1700,7 +1705,7 @@
       <c r="I7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="44" t="s">
+      <c r="J7" s="21" t="s">
         <v>135</v>
       </c>
       <c r="K7" s="6" t="s">
@@ -1713,23 +1718,23 @@
       <c r="N7" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="O7" s="50"/>
-      <c r="P7" s="50" t="s">
+      <c r="O7" s="27"/>
+      <c r="P7" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="46">
+      <c r="Q7" s="23">
         <v>6</v>
       </c>
-      <c r="R7" s="47" t="s">
+      <c r="R7" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S7" s="46" t="s">
+      <c r="S7" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T7" s="48" t="s">
+      <c r="T7" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="U7" s="46" t="s">
+      <c r="U7" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1743,12 +1748,12 @@
       <c r="C8" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="E8" s="49"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="43" t="s">
+      <c r="E8" s="26"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="20" t="s">
         <v>151</v>
       </c>
       <c r="H8" s="11">
@@ -1757,8 +1762,8 @@
       <c r="I8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="44" t="s">
-        <v>213</v>
+      <c r="J8" s="21" t="s">
+        <v>211</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>19</v>
@@ -1770,25 +1775,25 @@
         <v>117</v>
       </c>
       <c r="N8" s="7"/>
-      <c r="O8" s="50" t="s">
+      <c r="O8" s="27" t="s">
         <v>159</v>
       </c>
-      <c r="P8" s="50" t="s">
+      <c r="P8" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="46" t="s">
+      <c r="Q8" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="R8" s="47" t="s">
+      <c r="R8" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="S8" s="46" t="s">
+      <c r="S8" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="T8" s="48" t="s">
+      <c r="T8" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="U8" s="46" t="s">
+      <c r="U8" s="23" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1802,14 +1807,14 @@
       <c r="C9" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="E9" s="49" t="s">
+      <c r="E9" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="F9" s="50"/>
-      <c r="G9" s="43" t="s">
+      <c r="F9" s="27"/>
+      <c r="G9" s="20" t="s">
         <v>168</v>
       </c>
       <c r="H9" s="11">
@@ -1818,7 +1823,7 @@
       <c r="I9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="44" t="s">
+      <c r="J9" s="21" t="s">
         <v>171</v>
       </c>
       <c r="K9" s="6" t="s">
@@ -1831,23 +1836,23 @@
       <c r="N9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="O9" s="50"/>
-      <c r="P9" s="50" t="s">
+      <c r="O9" s="27"/>
+      <c r="P9" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="46">
+      <c r="Q9" s="23">
         <v>6</v>
       </c>
-      <c r="R9" s="47" t="s">
+      <c r="R9" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S9" s="46" t="s">
+      <c r="S9" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T9" s="48" t="s">
-        <v>222</v>
-      </c>
-      <c r="U9" s="46" t="s">
+      <c r="T9" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="U9" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1861,15 +1866,15 @@
       <c r="C10" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="E10" s="49" t="s">
+      <c r="E10" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="F10" s="50"/>
-      <c r="G10" s="43" t="s">
-        <v>208</v>
+      <c r="F10" s="27"/>
+      <c r="G10" s="20" t="s">
+        <v>206</v>
       </c>
       <c r="H10" s="11">
         <v>8</v>
@@ -1877,8 +1882,8 @@
       <c r="I10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="44" t="s">
-        <v>214</v>
+      <c r="J10" s="21" t="s">
+        <v>212</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>20</v>
@@ -1890,23 +1895,23 @@
       <c r="N10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="O10" s="50"/>
-      <c r="P10" s="50" t="s">
+      <c r="O10" s="27"/>
+      <c r="P10" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q10" s="46">
+      <c r="Q10" s="23">
         <v>6</v>
       </c>
-      <c r="R10" s="47" t="s">
+      <c r="R10" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S10" s="46" t="s">
+      <c r="S10" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T10" s="48" t="s">
+      <c r="T10" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="U10" s="46" t="s">
+      <c r="U10" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1920,14 +1925,14 @@
       <c r="C11" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="E11" s="49" t="s">
+      <c r="E11" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="F11" s="50"/>
-      <c r="G11" s="43" t="s">
+      <c r="F11" s="27"/>
+      <c r="G11" s="20" t="s">
         <v>136</v>
       </c>
       <c r="H11" s="11">
@@ -1936,7 +1941,7 @@
       <c r="I11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="44" t="s">
+      <c r="J11" s="21" t="s">
         <v>137</v>
       </c>
       <c r="K11" s="6" t="s">
@@ -1949,23 +1954,23 @@
       <c r="N11" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="O11" s="50"/>
-      <c r="P11" s="50" t="s">
+      <c r="O11" s="27"/>
+      <c r="P11" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="46">
+      <c r="Q11" s="23">
         <v>6</v>
       </c>
-      <c r="R11" s="47" t="s">
+      <c r="R11" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S11" s="46" t="s">
+      <c r="S11" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T11" s="48" t="s">
+      <c r="T11" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="U11" s="46" t="s">
+      <c r="U11" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1979,12 +1984,12 @@
       <c r="C12" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="E12" s="49"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="43" t="s">
+      <c r="E12" s="26"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="20" t="s">
         <v>147</v>
       </c>
       <c r="H12" s="15">
@@ -1993,8 +1998,8 @@
       <c r="I12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="44" t="s">
-        <v>223</v>
+      <c r="J12" s="21" t="s">
+        <v>229</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>20</v>
@@ -2004,26 +2009,26 @@
       </c>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
-      <c r="O12" s="50" t="s">
+      <c r="O12" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="P12" s="50" t="s">
+      <c r="P12" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="46">
+      <c r="Q12" s="23">
         <v>6</v>
       </c>
-      <c r="R12" s="47" t="s">
+      <c r="R12" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="S12" s="46" t="s">
-        <v>224</v>
-      </c>
-      <c r="T12" s="48" t="s">
-        <v>225</v>
-      </c>
-      <c r="U12" s="46" t="s">
-        <v>226</v>
+      <c r="S12" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="T12" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="U12" s="23" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2036,14 +2041,14 @@
       <c r="C13" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="E13" s="49" t="s">
+      <c r="E13" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="F13" s="50"/>
-      <c r="G13" s="43" t="s">
+      <c r="F13" s="27"/>
+      <c r="G13" s="20" t="s">
         <v>174</v>
       </c>
       <c r="H13" s="15">
@@ -2052,8 +2057,8 @@
       <c r="I13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="44" t="s">
-        <v>221</v>
+      <c r="J13" s="21" t="s">
+        <v>219</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>20</v>
@@ -2065,23 +2070,23 @@
       <c r="N13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="O13" s="50"/>
-      <c r="P13" s="50" t="s">
+      <c r="O13" s="27"/>
+      <c r="P13" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q13" s="46">
+      <c r="Q13" s="23">
         <v>6</v>
       </c>
-      <c r="R13" s="47" t="s">
+      <c r="R13" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S13" s="46" t="s">
+      <c r="S13" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T13" s="48" t="s">
+      <c r="T13" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="U13" s="46" t="s">
+      <c r="U13" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2095,14 +2100,14 @@
       <c r="C14" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="E14" s="49" t="s">
+      <c r="E14" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="F14" s="50"/>
-      <c r="G14" s="43" t="s">
+      <c r="F14" s="27"/>
+      <c r="G14" s="20" t="s">
         <v>176</v>
       </c>
       <c r="H14" s="15">
@@ -2111,7 +2116,7 @@
       <c r="I14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="44" t="s">
+      <c r="J14" s="21" t="s">
         <v>177</v>
       </c>
       <c r="K14" s="6" t="s">
@@ -2124,23 +2129,23 @@
       <c r="N14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="O14" s="50"/>
-      <c r="P14" s="50" t="s">
+      <c r="O14" s="27"/>
+      <c r="P14" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" s="46">
+      <c r="Q14" s="23">
         <v>6</v>
       </c>
-      <c r="R14" s="47" t="s">
+      <c r="R14" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S14" s="46" t="s">
+      <c r="S14" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T14" s="48" t="s">
+      <c r="T14" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="U14" s="46" t="s">
+      <c r="U14" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2154,14 +2159,14 @@
       <c r="C15" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="E15" s="49" t="s">
+      <c r="E15" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="F15" s="50"/>
-      <c r="G15" s="43" t="s">
+      <c r="F15" s="27"/>
+      <c r="G15" s="20" t="s">
         <v>178</v>
       </c>
       <c r="H15" s="15">
@@ -2170,8 +2175,8 @@
       <c r="I15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="44" t="s">
-        <v>215</v>
+      <c r="J15" s="21" t="s">
+        <v>213</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>20</v>
@@ -2183,23 +2188,23 @@
       <c r="N15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="O15" s="50"/>
-      <c r="P15" s="50" t="s">
+      <c r="O15" s="27"/>
+      <c r="P15" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="46">
+      <c r="Q15" s="23">
         <v>6</v>
       </c>
-      <c r="R15" s="47" t="s">
+      <c r="R15" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S15" s="46" t="s">
+      <c r="S15" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T15" s="48" t="s">
+      <c r="T15" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="U15" s="46" t="s">
+      <c r="U15" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2213,15 +2218,15 @@
       <c r="C16" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="E16" s="49" t="s">
+      <c r="E16" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="F16" s="50"/>
-      <c r="G16" s="43" t="s">
-        <v>211</v>
+      <c r="F16" s="27"/>
+      <c r="G16" s="20" t="s">
+        <v>209</v>
       </c>
       <c r="H16" s="15">
         <v>14</v>
@@ -2229,7 +2234,7 @@
       <c r="I16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="44" t="s">
+      <c r="J16" s="21" t="s">
         <v>186</v>
       </c>
       <c r="K16" s="6" t="s">
@@ -2242,23 +2247,23 @@
       <c r="N16" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="O16" s="50"/>
-      <c r="P16" s="50" t="s">
+      <c r="O16" s="27"/>
+      <c r="P16" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q16" s="46">
+      <c r="Q16" s="23">
         <v>6</v>
       </c>
-      <c r="R16" s="47" t="s">
+      <c r="R16" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S16" s="46" t="s">
+      <c r="S16" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T16" s="48" t="s">
+      <c r="T16" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="U16" s="46" t="s">
+      <c r="U16" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2272,14 +2277,14 @@
       <c r="C17" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="E17" s="49" t="s">
+      <c r="E17" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="F17" s="50"/>
-      <c r="G17" s="43" t="s">
+      <c r="F17" s="27"/>
+      <c r="G17" s="20" t="s">
         <v>138</v>
       </c>
       <c r="H17" s="15">
@@ -2288,7 +2293,7 @@
       <c r="I17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="44" t="s">
+      <c r="J17" s="21" t="s">
         <v>139</v>
       </c>
       <c r="K17" s="6" t="s">
@@ -2301,23 +2306,23 @@
       <c r="N17" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="O17" s="50"/>
-      <c r="P17" s="50" t="s">
+      <c r="O17" s="27"/>
+      <c r="P17" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q17" s="46">
+      <c r="Q17" s="23">
         <v>6</v>
       </c>
-      <c r="R17" s="47" t="s">
+      <c r="R17" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S17" s="46" t="s">
+      <c r="S17" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T17" s="48" t="s">
+      <c r="T17" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="U17" s="46" t="s">
+      <c r="U17" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2331,12 +2336,12 @@
       <c r="C18" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="E18" s="49"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="43" t="s">
+      <c r="E18" s="26"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="20" t="s">
         <v>148</v>
       </c>
       <c r="H18" s="16">
@@ -2345,7 +2350,7 @@
       <c r="I18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="44" t="s">
+      <c r="J18" s="21" t="s">
         <v>181</v>
       </c>
       <c r="K18" s="6" t="s">
@@ -2358,23 +2363,23 @@
         <v>117</v>
       </c>
       <c r="N18" s="7"/>
-      <c r="O18" s="50"/>
-      <c r="P18" s="50" t="s">
+      <c r="O18" s="27"/>
+      <c r="P18" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q18" s="46">
+      <c r="Q18" s="23">
         <v>6</v>
       </c>
-      <c r="R18" s="47" t="s">
+      <c r="R18" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S18" s="46" t="s">
+      <c r="S18" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="T18" s="48" t="s">
+      <c r="T18" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="U18" s="46" t="s">
+      <c r="U18" s="23" t="s">
         <v>184</v>
       </c>
     </row>
@@ -2388,28 +2393,28 @@
       <c r="C19" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="E19" s="49" t="s">
+      <c r="E19" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="F19" s="50"/>
-      <c r="G19" s="43"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="20"/>
       <c r="H19" s="15"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="44"/>
+      <c r="J19" s="21"/>
       <c r="K19" s="6"/>
       <c r="L19" s="5"/>
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
-      <c r="O19" s="50"/>
-      <c r="P19" s="50"/>
-      <c r="Q19" s="46"/>
-      <c r="R19" s="47"/>
-      <c r="S19" s="46"/>
-      <c r="T19" s="48"/>
-      <c r="U19" s="46"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="27"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="24"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="25"/>
+      <c r="U19" s="23"/>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
@@ -2421,28 +2426,28 @@
       <c r="C20" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="E20" s="49" t="s">
-        <v>216</v>
-      </c>
-      <c r="F20" s="50"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="50"/>
+      <c r="E20" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="F20" s="27"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="27"/>
       <c r="I20" s="4"/>
-      <c r="J20" s="44"/>
+      <c r="J20" s="21"/>
       <c r="K20" s="6"/>
       <c r="L20" s="5"/>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
-      <c r="O20" s="50"/>
-      <c r="P20" s="50"/>
-      <c r="Q20" s="46"/>
-      <c r="R20" s="47"/>
-      <c r="S20" s="46"/>
-      <c r="T20" s="48"/>
-      <c r="U20" s="46"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="25"/>
+      <c r="U20" s="23"/>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
@@ -2454,14 +2459,14 @@
       <c r="C21" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="E21" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="F21" s="50"/>
-      <c r="G21" s="43" t="s">
+      <c r="E21" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="F21" s="27"/>
+      <c r="G21" s="20" t="s">
         <v>149</v>
       </c>
       <c r="H21" s="15">
@@ -2470,8 +2475,8 @@
       <c r="I21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="44" t="s">
-        <v>218</v>
+      <c r="J21" s="21" t="s">
+        <v>216</v>
       </c>
       <c r="K21" s="6" t="s">
         <v>20</v>
@@ -2481,26 +2486,26 @@
       </c>
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
-      <c r="O21" s="50" t="s">
+      <c r="O21" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="P21" s="50" t="s">
+      <c r="P21" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q21" s="46">
+      <c r="Q21" s="23">
         <v>6</v>
       </c>
-      <c r="R21" s="47" t="s">
+      <c r="R21" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="S21" s="46" t="s">
+      <c r="S21" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="T21" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="T21" s="48" t="s">
-        <v>227</v>
-      </c>
-      <c r="U21" s="46" t="s">
-        <v>226</v>
+      <c r="U21" s="23" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2513,14 +2518,14 @@
       <c r="C22" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D22" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="E22" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="F22" s="50"/>
-      <c r="G22" s="43" t="s">
+      <c r="E22" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="F22" s="27"/>
+      <c r="G22" s="20" t="s">
         <v>185</v>
       </c>
       <c r="H22" s="15">
@@ -2529,7 +2534,7 @@
       <c r="I22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="44" t="s">
+      <c r="J22" s="21" t="s">
         <v>188</v>
       </c>
       <c r="K22" s="6" t="s">
@@ -2542,23 +2547,23 @@
       <c r="N22" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="O22" s="50"/>
-      <c r="P22" s="50" t="s">
+      <c r="O22" s="27"/>
+      <c r="P22" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q22" s="46">
+      <c r="Q22" s="23">
         <v>6</v>
       </c>
-      <c r="R22" s="47" t="s">
+      <c r="R22" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S22" s="46" t="s">
+      <c r="S22" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T22" s="48" t="s">
+      <c r="T22" s="25" t="s">
         <v>189</v>
       </c>
-      <c r="U22" s="46" t="s">
+      <c r="U22" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2572,14 +2577,14 @@
       <c r="C23" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="42" t="s">
+      <c r="D23" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="E23" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="F23" s="50"/>
-      <c r="G23" s="43" t="s">
+      <c r="E23" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="F23" s="27"/>
+      <c r="G23" s="20" t="s">
         <v>191</v>
       </c>
       <c r="H23" s="15">
@@ -2588,7 +2593,7 @@
       <c r="I23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="44" t="s">
+      <c r="J23" s="21" t="s">
         <v>192</v>
       </c>
       <c r="K23" s="6" t="s">
@@ -2601,23 +2606,23 @@
       <c r="N23" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="O23" s="50"/>
-      <c r="P23" s="50" t="s">
+      <c r="O23" s="27"/>
+      <c r="P23" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="46">
+      <c r="Q23" s="23">
         <v>6</v>
       </c>
-      <c r="R23" s="47" t="s">
+      <c r="R23" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S23" s="46" t="s">
+      <c r="S23" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T23" s="48" t="s">
+      <c r="T23" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="U23" s="46" t="s">
+      <c r="U23" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2631,14 +2636,14 @@
       <c r="C24" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D24" s="42" t="s">
+      <c r="D24" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="E24" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="F24" s="50"/>
-      <c r="G24" s="43" t="s">
+      <c r="E24" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="F24" s="27"/>
+      <c r="G24" s="20" t="s">
         <v>195</v>
       </c>
       <c r="H24" s="15">
@@ -2647,7 +2652,7 @@
       <c r="I24" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="44" t="s">
+      <c r="J24" s="21" t="s">
         <v>193</v>
       </c>
       <c r="K24" s="6" t="s">
@@ -2660,23 +2665,23 @@
       <c r="N24" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="O24" s="50"/>
-      <c r="P24" s="50" t="s">
+      <c r="O24" s="27"/>
+      <c r="P24" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q24" s="46">
+      <c r="Q24" s="23">
         <v>6</v>
       </c>
-      <c r="R24" s="47" t="s">
+      <c r="R24" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S24" s="46" t="s">
+      <c r="S24" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T24" s="48" t="s">
+      <c r="T24" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="U24" s="46" t="s">
+      <c r="U24" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2690,15 +2695,15 @@
       <c r="C25" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="42" t="s">
+      <c r="D25" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="E25" s="49" t="s">
+      <c r="E25" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="F25" s="27"/>
+      <c r="G25" s="20" t="s">
         <v>217</v>
-      </c>
-      <c r="F25" s="50"/>
-      <c r="G25" s="43" t="s">
-        <v>219</v>
       </c>
       <c r="H25" s="15">
         <v>21</v>
@@ -2706,8 +2711,8 @@
       <c r="I25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="44" t="s">
-        <v>229</v>
+      <c r="J25" s="21" t="s">
+        <v>226</v>
       </c>
       <c r="K25" s="6" t="s">
         <v>20</v>
@@ -2719,23 +2724,23 @@
       <c r="N25" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="O25" s="50"/>
-      <c r="P25" s="50" t="s">
+      <c r="O25" s="27"/>
+      <c r="P25" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q25" s="46">
+      <c r="Q25" s="23">
         <v>6</v>
       </c>
-      <c r="R25" s="47" t="s">
+      <c r="R25" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S25" s="46" t="s">
+      <c r="S25" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T25" s="48" t="s">
-        <v>200</v>
-      </c>
-      <c r="U25" s="46" t="s">
+      <c r="T25" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="U25" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2749,14 +2754,14 @@
       <c r="C26" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D26" s="42" t="s">
+      <c r="D26" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="E26" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="F26" s="50"/>
-      <c r="G26" s="43" t="s">
+      <c r="E26" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="F26" s="27"/>
+      <c r="G26" s="20" t="s">
         <v>140</v>
       </c>
       <c r="H26" s="15">
@@ -2765,7 +2770,7 @@
       <c r="I26" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="44" t="s">
+      <c r="J26" s="21" t="s">
         <v>141</v>
       </c>
       <c r="K26" s="6" t="s">
@@ -2778,21 +2783,21 @@
       <c r="N26" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="O26" s="50"/>
-      <c r="P26" s="50"/>
-      <c r="Q26" s="46">
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
+      <c r="Q26" s="23">
         <v>6</v>
       </c>
-      <c r="R26" s="47" t="s">
+      <c r="R26" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S26" s="46" t="s">
+      <c r="S26" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T26" s="48" t="s">
+      <c r="T26" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="U26" s="46" t="s">
+      <c r="U26" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2806,13 +2811,13 @@
       <c r="C27" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D27" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="E27" s="49"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="43" t="s">
-        <v>197</v>
+      <c r="E27" s="26"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="20" t="s">
+        <v>230</v>
       </c>
       <c r="H27" s="15">
         <v>23</v>
@@ -2820,8 +2825,8 @@
       <c r="I27" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="44" t="s">
-        <v>198</v>
+      <c r="J27" s="21" t="s">
+        <v>231</v>
       </c>
       <c r="K27" s="6" t="s">
         <v>20</v>
@@ -2833,23 +2838,23 @@
       <c r="N27" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="O27" s="50"/>
-      <c r="P27" s="50" t="s">
+      <c r="O27" s="27"/>
+      <c r="P27" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="46">
+      <c r="Q27" s="23">
         <v>6</v>
       </c>
-      <c r="R27" s="47" t="s">
+      <c r="R27" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S27" s="46" t="s">
+      <c r="S27" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T27" s="48" t="s">
-        <v>199</v>
-      </c>
-      <c r="U27" s="46" t="s">
+      <c r="T27" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="U27" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2863,13 +2868,13 @@
       <c r="C28" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D28" s="42" t="s">
+      <c r="D28" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="E28" s="49"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="43" t="s">
-        <v>228</v>
+      <c r="E28" s="26"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="20" t="s">
+        <v>225</v>
       </c>
       <c r="H28" s="15">
         <v>24</v>
@@ -2877,8 +2882,8 @@
       <c r="I28" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="44" t="s">
-        <v>231</v>
+      <c r="J28" s="21" t="s">
+        <v>228</v>
       </c>
       <c r="K28" s="6" t="s">
         <v>20</v>
@@ -2890,23 +2895,23 @@
       <c r="N28" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="O28" s="50"/>
-      <c r="P28" s="50" t="s">
+      <c r="O28" s="27"/>
+      <c r="P28" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q28" s="46">
+      <c r="Q28" s="23">
         <v>6</v>
       </c>
-      <c r="R28" s="47" t="s">
+      <c r="R28" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S28" s="46" t="s">
+      <c r="S28" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T28" s="48" t="s">
-        <v>230</v>
-      </c>
-      <c r="U28" s="46" t="s">
+      <c r="T28" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="U28" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2920,12 +2925,12 @@
       <c r="C29" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D29" s="42" t="s">
-        <v>202</v>
-      </c>
-      <c r="E29" s="49"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="43" t="s">
+      <c r="D29" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="E29" s="26"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="20" t="s">
         <v>10</v>
       </c>
       <c r="H29" s="15">
@@ -2934,8 +2939,8 @@
       <c r="I29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="44" t="s">
-        <v>203</v>
+      <c r="J29" s="21" t="s">
+        <v>201</v>
       </c>
       <c r="K29" s="6" t="s">
         <v>20</v>
@@ -2945,15 +2950,15 @@
       </c>
       <c r="M29" s="7"/>
       <c r="N29" s="7"/>
-      <c r="O29" s="50"/>
-      <c r="P29" s="50" t="s">
+      <c r="O29" s="27"/>
+      <c r="P29" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q29" s="46"/>
-      <c r="R29" s="47"/>
-      <c r="S29" s="46"/>
-      <c r="T29" s="48"/>
-      <c r="U29" s="46"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="24"/>
+      <c r="S29" s="23"/>
+      <c r="T29" s="25"/>
+      <c r="U29" s="23"/>
     </row>
     <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
@@ -2965,13 +2970,13 @@
       <c r="C30" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D30" s="42" t="s">
-        <v>202</v>
-      </c>
-      <c r="E30" s="49"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="43" t="s">
-        <v>201</v>
+      <c r="D30" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="E30" s="26"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="20" t="s">
+        <v>199</v>
       </c>
       <c r="H30" s="15">
         <v>26</v>
@@ -2979,8 +2984,8 @@
       <c r="I30" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J30" s="44" t="s">
-        <v>204</v>
+      <c r="J30" s="21" t="s">
+        <v>202</v>
       </c>
       <c r="K30" s="6" t="s">
         <v>20</v>
@@ -2992,23 +2997,23 @@
       <c r="N30" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="O30" s="50"/>
-      <c r="P30" s="50" t="s">
+      <c r="O30" s="27"/>
+      <c r="P30" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q30" s="46">
+      <c r="Q30" s="23">
         <v>6</v>
       </c>
-      <c r="R30" s="47" t="s">
+      <c r="R30" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S30" s="46" t="s">
+      <c r="S30" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T30" s="48" t="s">
-        <v>206</v>
-      </c>
-      <c r="U30" s="46" t="s">
+      <c r="T30" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="U30" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3022,13 +3027,13 @@
       <c r="C31" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D31" s="42" t="s">
-        <v>202</v>
-      </c>
-      <c r="E31" s="49"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="43" t="s">
-        <v>220</v>
+      <c r="D31" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="E31" s="26"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="20" t="s">
+        <v>218</v>
       </c>
       <c r="H31" s="15">
         <v>27</v>
@@ -3036,8 +3041,8 @@
       <c r="I31" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J31" s="44" t="s">
-        <v>205</v>
+      <c r="J31" s="21" t="s">
+        <v>203</v>
       </c>
       <c r="K31" s="6" t="s">
         <v>20</v>
@@ -3049,1198 +3054,1198 @@
       <c r="N31" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="O31" s="50"/>
-      <c r="P31" s="50" t="s">
+      <c r="O31" s="27"/>
+      <c r="P31" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q31" s="46">
+      <c r="Q31" s="23">
         <v>6</v>
       </c>
-      <c r="R31" s="47" t="s">
+      <c r="R31" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S31" s="46" t="s">
+      <c r="S31" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="T31" s="48" t="s">
-        <v>207</v>
-      </c>
-      <c r="U31" s="46" t="s">
+      <c r="T31" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="U31" s="23" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
-      <c r="B32" s="49"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="50"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="27"/>
       <c r="I32" s="4"/>
-      <c r="J32" s="44"/>
+      <c r="J32" s="21"/>
       <c r="K32" s="6"/>
       <c r="L32" s="5"/>
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
-      <c r="O32" s="50"/>
-      <c r="P32" s="50"/>
-      <c r="Q32" s="46"/>
-      <c r="R32" s="47"/>
-      <c r="S32" s="46"/>
-      <c r="T32" s="48"/>
-      <c r="U32" s="46"/>
+      <c r="O32" s="27"/>
+      <c r="P32" s="27"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="24"/>
+      <c r="S32" s="23"/>
+      <c r="T32" s="25"/>
+      <c r="U32" s="23"/>
     </row>
     <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
-      <c r="B33" s="49"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="50"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="27"/>
       <c r="I33" s="4"/>
-      <c r="J33" s="44"/>
+      <c r="J33" s="21"/>
       <c r="K33" s="6"/>
       <c r="L33" s="5"/>
       <c r="M33" s="7"/>
       <c r="N33" s="7"/>
-      <c r="O33" s="50"/>
-      <c r="P33" s="50"/>
-      <c r="Q33" s="46"/>
-      <c r="R33" s="47"/>
-      <c r="S33" s="46"/>
-      <c r="T33" s="48"/>
-      <c r="U33" s="46"/>
+      <c r="O33" s="27"/>
+      <c r="P33" s="27"/>
+      <c r="Q33" s="23"/>
+      <c r="R33" s="24"/>
+      <c r="S33" s="23"/>
+      <c r="T33" s="25"/>
+      <c r="U33" s="23"/>
     </row>
     <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
-      <c r="B34" s="49"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="49"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="50"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="27"/>
       <c r="I34" s="4"/>
-      <c r="J34" s="44"/>
+      <c r="J34" s="21"/>
       <c r="K34" s="6"/>
       <c r="L34" s="5"/>
       <c r="M34" s="7"/>
       <c r="N34" s="7"/>
-      <c r="O34" s="50"/>
-      <c r="P34" s="50"/>
-      <c r="Q34" s="46"/>
-      <c r="R34" s="47"/>
-      <c r="S34" s="46"/>
-      <c r="T34" s="48"/>
-      <c r="U34" s="46"/>
+      <c r="O34" s="27"/>
+      <c r="P34" s="27"/>
+      <c r="Q34" s="23"/>
+      <c r="R34" s="24"/>
+      <c r="S34" s="23"/>
+      <c r="T34" s="25"/>
+      <c r="U34" s="23"/>
     </row>
     <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
-      <c r="B35" s="49"/>
-      <c r="C35" s="51"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="50"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="27"/>
       <c r="I35" s="4"/>
-      <c r="J35" s="44"/>
+      <c r="J35" s="21"/>
       <c r="K35" s="6"/>
       <c r="L35" s="5"/>
       <c r="M35" s="7"/>
       <c r="N35" s="7"/>
-      <c r="O35" s="50"/>
-      <c r="P35" s="50"/>
-      <c r="Q35" s="46"/>
-      <c r="R35" s="47"/>
-      <c r="S35" s="46"/>
-      <c r="T35" s="48"/>
-      <c r="U35" s="46"/>
+      <c r="O35" s="27"/>
+      <c r="P35" s="27"/>
+      <c r="Q35" s="23"/>
+      <c r="R35" s="24"/>
+      <c r="S35" s="23"/>
+      <c r="T35" s="25"/>
+      <c r="U35" s="23"/>
     </row>
     <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
-      <c r="B36" s="49"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="50"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="50"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="27"/>
       <c r="I36" s="4"/>
-      <c r="J36" s="44"/>
+      <c r="J36" s="21"/>
       <c r="K36" s="6"/>
       <c r="L36" s="5"/>
       <c r="M36" s="7"/>
       <c r="N36" s="7"/>
-      <c r="O36" s="50"/>
-      <c r="P36" s="50"/>
-      <c r="Q36" s="46"/>
-      <c r="R36" s="47"/>
-      <c r="S36" s="46"/>
-      <c r="T36" s="48"/>
-      <c r="U36" s="46"/>
+      <c r="O36" s="27"/>
+      <c r="P36" s="27"/>
+      <c r="Q36" s="23"/>
+      <c r="R36" s="24"/>
+      <c r="S36" s="23"/>
+      <c r="T36" s="25"/>
+      <c r="U36" s="23"/>
     </row>
     <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
-      <c r="B37" s="49"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="50"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="50"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="27"/>
       <c r="I37" s="4"/>
-      <c r="J37" s="44"/>
+      <c r="J37" s="21"/>
       <c r="K37" s="6"/>
       <c r="L37" s="5"/>
       <c r="M37" s="7"/>
       <c r="N37" s="7"/>
-      <c r="O37" s="50"/>
-      <c r="P37" s="50"/>
-      <c r="Q37" s="46"/>
-      <c r="R37" s="47"/>
-      <c r="S37" s="46"/>
-      <c r="T37" s="48"/>
-      <c r="U37" s="46"/>
+      <c r="O37" s="27"/>
+      <c r="P37" s="27"/>
+      <c r="Q37" s="23"/>
+      <c r="R37" s="24"/>
+      <c r="S37" s="23"/>
+      <c r="T37" s="25"/>
+      <c r="U37" s="23"/>
     </row>
     <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
-      <c r="B38" s="49"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="49"/>
-      <c r="F38" s="50"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="50"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="27"/>
       <c r="I38" s="4"/>
-      <c r="J38" s="44"/>
+      <c r="J38" s="21"/>
       <c r="K38" s="6"/>
       <c r="L38" s="5"/>
       <c r="M38" s="7"/>
       <c r="N38" s="7"/>
-      <c r="O38" s="50"/>
-      <c r="P38" s="50"/>
-      <c r="Q38" s="46"/>
-      <c r="R38" s="47"/>
-      <c r="S38" s="46"/>
-      <c r="T38" s="48"/>
-      <c r="U38" s="46"/>
+      <c r="O38" s="27"/>
+      <c r="P38" s="27"/>
+      <c r="Q38" s="23"/>
+      <c r="R38" s="24"/>
+      <c r="S38" s="23"/>
+      <c r="T38" s="25"/>
+      <c r="U38" s="23"/>
     </row>
     <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
-      <c r="B39" s="49"/>
-      <c r="C39" s="51"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="50"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="50"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="27"/>
       <c r="I39" s="4"/>
-      <c r="J39" s="44"/>
+      <c r="J39" s="21"/>
       <c r="K39" s="6"/>
       <c r="L39" s="5"/>
       <c r="M39" s="7"/>
       <c r="N39" s="7"/>
-      <c r="O39" s="50"/>
-      <c r="P39" s="50"/>
-      <c r="Q39" s="46"/>
-      <c r="R39" s="47"/>
-      <c r="S39" s="46"/>
-      <c r="T39" s="48"/>
-      <c r="U39" s="46"/>
+      <c r="O39" s="27"/>
+      <c r="P39" s="27"/>
+      <c r="Q39" s="23"/>
+      <c r="R39" s="24"/>
+      <c r="S39" s="23"/>
+      <c r="T39" s="25"/>
+      <c r="U39" s="23"/>
     </row>
     <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
-      <c r="B40" s="49"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="49"/>
-      <c r="F40" s="50"/>
-      <c r="G40" s="43"/>
-      <c r="H40" s="50"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="27"/>
       <c r="I40" s="4"/>
-      <c r="J40" s="44"/>
+      <c r="J40" s="21"/>
       <c r="K40" s="6"/>
       <c r="L40" s="5"/>
       <c r="M40" s="7"/>
       <c r="N40" s="7"/>
-      <c r="O40" s="50"/>
-      <c r="P40" s="50"/>
-      <c r="Q40" s="46"/>
-      <c r="R40" s="47"/>
-      <c r="S40" s="46"/>
-      <c r="T40" s="48"/>
-      <c r="U40" s="46"/>
+      <c r="O40" s="27"/>
+      <c r="P40" s="27"/>
+      <c r="Q40" s="23"/>
+      <c r="R40" s="24"/>
+      <c r="S40" s="23"/>
+      <c r="T40" s="25"/>
+      <c r="U40" s="23"/>
     </row>
     <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
-      <c r="B41" s="49"/>
-      <c r="C41" s="51"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="49"/>
-      <c r="F41" s="50"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="50"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="27"/>
       <c r="I41" s="4"/>
-      <c r="J41" s="44"/>
+      <c r="J41" s="21"/>
       <c r="K41" s="6"/>
       <c r="L41" s="5"/>
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
-      <c r="O41" s="50"/>
-      <c r="P41" s="50"/>
-      <c r="Q41" s="46"/>
-      <c r="R41" s="47"/>
-      <c r="S41" s="46"/>
-      <c r="T41" s="48"/>
-      <c r="U41" s="46"/>
+      <c r="O41" s="27"/>
+      <c r="P41" s="27"/>
+      <c r="Q41" s="23"/>
+      <c r="R41" s="24"/>
+      <c r="S41" s="23"/>
+      <c r="T41" s="25"/>
+      <c r="U41" s="23"/>
     </row>
     <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
-      <c r="B42" s="49"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="49"/>
-      <c r="F42" s="50"/>
-      <c r="G42" s="43"/>
-      <c r="H42" s="50"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="27"/>
       <c r="I42" s="4"/>
-      <c r="J42" s="44"/>
+      <c r="J42" s="21"/>
       <c r="K42" s="6"/>
       <c r="L42" s="5"/>
       <c r="M42" s="7"/>
       <c r="N42" s="7"/>
-      <c r="O42" s="50"/>
-      <c r="P42" s="50"/>
-      <c r="Q42" s="46"/>
-      <c r="R42" s="47"/>
-      <c r="S42" s="46"/>
-      <c r="T42" s="48"/>
-      <c r="U42" s="46"/>
+      <c r="O42" s="27"/>
+      <c r="P42" s="27"/>
+      <c r="Q42" s="23"/>
+      <c r="R42" s="24"/>
+      <c r="S42" s="23"/>
+      <c r="T42" s="25"/>
+      <c r="U42" s="23"/>
     </row>
     <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
-      <c r="B43" s="49"/>
-      <c r="C43" s="51"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="49"/>
-      <c r="F43" s="50"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="50"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="27"/>
       <c r="I43" s="4"/>
-      <c r="J43" s="44"/>
+      <c r="J43" s="21"/>
       <c r="K43" s="6"/>
       <c r="L43" s="5"/>
       <c r="M43" s="7"/>
       <c r="N43" s="7"/>
-      <c r="O43" s="50"/>
-      <c r="P43" s="50"/>
-      <c r="Q43" s="46"/>
-      <c r="R43" s="47"/>
-      <c r="S43" s="46"/>
-      <c r="T43" s="48"/>
-      <c r="U43" s="46"/>
+      <c r="O43" s="27"/>
+      <c r="P43" s="27"/>
+      <c r="Q43" s="23"/>
+      <c r="R43" s="24"/>
+      <c r="S43" s="23"/>
+      <c r="T43" s="25"/>
+      <c r="U43" s="23"/>
     </row>
     <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
-      <c r="B44" s="49"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="49"/>
-      <c r="F44" s="50"/>
-      <c r="G44" s="43"/>
-      <c r="H44" s="50"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="27"/>
       <c r="I44" s="4"/>
-      <c r="J44" s="44"/>
+      <c r="J44" s="21"/>
       <c r="K44" s="6"/>
       <c r="L44" s="5"/>
       <c r="M44" s="7"/>
       <c r="N44" s="7"/>
-      <c r="O44" s="50"/>
-      <c r="P44" s="50"/>
-      <c r="Q44" s="46"/>
-      <c r="R44" s="47"/>
-      <c r="S44" s="46"/>
-      <c r="T44" s="48"/>
-      <c r="U44" s="46"/>
+      <c r="O44" s="27"/>
+      <c r="P44" s="27"/>
+      <c r="Q44" s="23"/>
+      <c r="R44" s="24"/>
+      <c r="S44" s="23"/>
+      <c r="T44" s="25"/>
+      <c r="U44" s="23"/>
     </row>
     <row r="45" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
-      <c r="B45" s="49"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="49"/>
-      <c r="F45" s="50"/>
-      <c r="G45" s="43"/>
-      <c r="H45" s="50"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="27"/>
       <c r="I45" s="4"/>
-      <c r="J45" s="44"/>
+      <c r="J45" s="21"/>
       <c r="K45" s="6"/>
       <c r="L45" s="5"/>
       <c r="M45" s="7"/>
       <c r="N45" s="7"/>
-      <c r="O45" s="50"/>
-      <c r="P45" s="50"/>
-      <c r="Q45" s="46"/>
-      <c r="R45" s="47"/>
-      <c r="S45" s="46"/>
-      <c r="T45" s="48"/>
-      <c r="U45" s="46"/>
+      <c r="O45" s="27"/>
+      <c r="P45" s="27"/>
+      <c r="Q45" s="23"/>
+      <c r="R45" s="24"/>
+      <c r="S45" s="23"/>
+      <c r="T45" s="25"/>
+      <c r="U45" s="23"/>
     </row>
     <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
-      <c r="B46" s="49"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="49"/>
-      <c r="F46" s="50"/>
-      <c r="G46" s="43"/>
-      <c r="H46" s="50"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="27"/>
       <c r="I46" s="4"/>
-      <c r="J46" s="44"/>
+      <c r="J46" s="21"/>
       <c r="K46" s="6"/>
       <c r="L46" s="5"/>
       <c r="M46" s="7"/>
       <c r="N46" s="7"/>
-      <c r="O46" s="50"/>
-      <c r="P46" s="50"/>
-      <c r="Q46" s="46"/>
-      <c r="R46" s="47"/>
-      <c r="S46" s="46"/>
-      <c r="T46" s="48"/>
-      <c r="U46" s="46"/>
+      <c r="O46" s="27"/>
+      <c r="P46" s="27"/>
+      <c r="Q46" s="23"/>
+      <c r="R46" s="24"/>
+      <c r="S46" s="23"/>
+      <c r="T46" s="25"/>
+      <c r="U46" s="23"/>
     </row>
     <row r="47" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
-      <c r="B47" s="49"/>
-      <c r="C47" s="51"/>
-      <c r="D47" s="42"/>
-      <c r="E47" s="49"/>
-      <c r="F47" s="50"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="50"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="27"/>
       <c r="I47" s="4"/>
-      <c r="J47" s="44"/>
+      <c r="J47" s="21"/>
       <c r="K47" s="6"/>
       <c r="L47" s="5"/>
       <c r="M47" s="7"/>
       <c r="N47" s="7"/>
-      <c r="O47" s="50"/>
-      <c r="P47" s="50"/>
-      <c r="Q47" s="46"/>
-      <c r="R47" s="47"/>
-      <c r="S47" s="46"/>
-      <c r="T47" s="48"/>
-      <c r="U47" s="46"/>
+      <c r="O47" s="27"/>
+      <c r="P47" s="27"/>
+      <c r="Q47" s="23"/>
+      <c r="R47" s="24"/>
+      <c r="S47" s="23"/>
+      <c r="T47" s="25"/>
+      <c r="U47" s="23"/>
     </row>
     <row r="48" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
-      <c r="B48" s="49"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="42"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="50"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="50"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="27"/>
       <c r="I48" s="4"/>
-      <c r="J48" s="44"/>
+      <c r="J48" s="21"/>
       <c r="K48" s="6"/>
       <c r="L48" s="5"/>
       <c r="M48" s="7"/>
       <c r="N48" s="7"/>
-      <c r="O48" s="50"/>
-      <c r="P48" s="50"/>
-      <c r="Q48" s="46"/>
-      <c r="R48" s="47"/>
-      <c r="S48" s="46"/>
-      <c r="T48" s="48"/>
-      <c r="U48" s="46"/>
+      <c r="O48" s="27"/>
+      <c r="P48" s="27"/>
+      <c r="Q48" s="23"/>
+      <c r="R48" s="24"/>
+      <c r="S48" s="23"/>
+      <c r="T48" s="25"/>
+      <c r="U48" s="23"/>
     </row>
     <row r="49" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
-      <c r="B49" s="49"/>
-      <c r="C49" s="51"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="49"/>
-      <c r="F49" s="50"/>
-      <c r="G49" s="43"/>
-      <c r="H49" s="50"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="27"/>
       <c r="I49" s="4"/>
-      <c r="J49" s="44"/>
+      <c r="J49" s="21"/>
       <c r="K49" s="6"/>
       <c r="L49" s="5"/>
       <c r="M49" s="7"/>
       <c r="N49" s="7"/>
-      <c r="O49" s="50"/>
-      <c r="P49" s="50"/>
-      <c r="Q49" s="46"/>
-      <c r="R49" s="47"/>
-      <c r="S49" s="46"/>
-      <c r="T49" s="48"/>
-      <c r="U49" s="46"/>
+      <c r="O49" s="27"/>
+      <c r="P49" s="27"/>
+      <c r="Q49" s="23"/>
+      <c r="R49" s="24"/>
+      <c r="S49" s="23"/>
+      <c r="T49" s="25"/>
+      <c r="U49" s="23"/>
     </row>
     <row r="50" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
-      <c r="B50" s="49"/>
-      <c r="C50" s="51"/>
-      <c r="D50" s="42"/>
-      <c r="E50" s="49"/>
-      <c r="F50" s="50"/>
-      <c r="G50" s="43"/>
-      <c r="H50" s="50"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="27"/>
       <c r="I50" s="4"/>
-      <c r="J50" s="44"/>
+      <c r="J50" s="21"/>
       <c r="K50" s="6"/>
       <c r="L50" s="5"/>
       <c r="M50" s="7"/>
       <c r="N50" s="7"/>
-      <c r="O50" s="50"/>
-      <c r="P50" s="50"/>
-      <c r="Q50" s="46"/>
-      <c r="R50" s="47"/>
-      <c r="S50" s="46"/>
-      <c r="T50" s="48"/>
-      <c r="U50" s="46"/>
+      <c r="O50" s="27"/>
+      <c r="P50" s="27"/>
+      <c r="Q50" s="23"/>
+      <c r="R50" s="24"/>
+      <c r="S50" s="23"/>
+      <c r="T50" s="25"/>
+      <c r="U50" s="23"/>
     </row>
     <row r="51" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
-      <c r="B51" s="49"/>
-      <c r="C51" s="51"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="49"/>
-      <c r="F51" s="50"/>
-      <c r="G51" s="43"/>
-      <c r="H51" s="50"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="27"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="27"/>
       <c r="I51" s="4"/>
-      <c r="J51" s="44"/>
+      <c r="J51" s="21"/>
       <c r="K51" s="6"/>
       <c r="L51" s="5"/>
       <c r="M51" s="7"/>
       <c r="N51" s="7"/>
-      <c r="O51" s="50"/>
-      <c r="P51" s="50"/>
-      <c r="Q51" s="46"/>
-      <c r="R51" s="47"/>
-      <c r="S51" s="46"/>
-      <c r="T51" s="48"/>
-      <c r="U51" s="46"/>
+      <c r="O51" s="27"/>
+      <c r="P51" s="27"/>
+      <c r="Q51" s="23"/>
+      <c r="R51" s="24"/>
+      <c r="S51" s="23"/>
+      <c r="T51" s="25"/>
+      <c r="U51" s="23"/>
     </row>
     <row r="52" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
-      <c r="B52" s="49"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="42"/>
-      <c r="E52" s="49"/>
-      <c r="F52" s="50"/>
-      <c r="G52" s="43"/>
-      <c r="H52" s="50"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="27"/>
       <c r="I52" s="4"/>
-      <c r="J52" s="44"/>
+      <c r="J52" s="21"/>
       <c r="K52" s="6"/>
       <c r="L52" s="5"/>
       <c r="M52" s="7"/>
       <c r="N52" s="7"/>
-      <c r="O52" s="50"/>
-      <c r="P52" s="50"/>
-      <c r="Q52" s="46"/>
-      <c r="R52" s="47"/>
-      <c r="S52" s="46"/>
-      <c r="T52" s="48"/>
-      <c r="U52" s="46"/>
+      <c r="O52" s="27"/>
+      <c r="P52" s="27"/>
+      <c r="Q52" s="23"/>
+      <c r="R52" s="24"/>
+      <c r="S52" s="23"/>
+      <c r="T52" s="25"/>
+      <c r="U52" s="23"/>
     </row>
     <row r="53" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
-      <c r="B53" s="49"/>
-      <c r="C53" s="51"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="49"/>
-      <c r="F53" s="50"/>
-      <c r="G53" s="43"/>
-      <c r="H53" s="50"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="27"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="27"/>
       <c r="I53" s="4"/>
-      <c r="J53" s="44"/>
+      <c r="J53" s="21"/>
       <c r="K53" s="6"/>
       <c r="L53" s="5"/>
       <c r="M53" s="7"/>
       <c r="N53" s="7"/>
-      <c r="O53" s="50"/>
-      <c r="P53" s="50"/>
-      <c r="Q53" s="46"/>
-      <c r="R53" s="47"/>
-      <c r="S53" s="46"/>
-      <c r="T53" s="48"/>
-      <c r="U53" s="46"/>
+      <c r="O53" s="27"/>
+      <c r="P53" s="27"/>
+      <c r="Q53" s="23"/>
+      <c r="R53" s="24"/>
+      <c r="S53" s="23"/>
+      <c r="T53" s="25"/>
+      <c r="U53" s="23"/>
     </row>
     <row r="54" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
-      <c r="B54" s="49"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="49"/>
-      <c r="F54" s="50"/>
-      <c r="G54" s="43"/>
-      <c r="H54" s="50"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="27"/>
+      <c r="G54" s="20"/>
+      <c r="H54" s="27"/>
       <c r="I54" s="4"/>
-      <c r="J54" s="44"/>
+      <c r="J54" s="21"/>
       <c r="K54" s="6"/>
       <c r="L54" s="5"/>
       <c r="M54" s="7"/>
       <c r="N54" s="7"/>
-      <c r="O54" s="50"/>
-      <c r="P54" s="50"/>
-      <c r="Q54" s="46"/>
-      <c r="R54" s="47"/>
-      <c r="S54" s="46"/>
-      <c r="T54" s="48"/>
-      <c r="U54" s="46"/>
+      <c r="O54" s="27"/>
+      <c r="P54" s="27"/>
+      <c r="Q54" s="23"/>
+      <c r="R54" s="24"/>
+      <c r="S54" s="23"/>
+      <c r="T54" s="25"/>
+      <c r="U54" s="23"/>
     </row>
     <row r="55" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
-      <c r="B55" s="49"/>
-      <c r="C55" s="51"/>
-      <c r="D55" s="42"/>
-      <c r="E55" s="49"/>
-      <c r="F55" s="50"/>
-      <c r="G55" s="43"/>
-      <c r="H55" s="50"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="27"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="27"/>
       <c r="I55" s="4"/>
-      <c r="J55" s="44"/>
+      <c r="J55" s="21"/>
       <c r="K55" s="6"/>
       <c r="L55" s="5"/>
       <c r="M55" s="7"/>
       <c r="N55" s="7"/>
-      <c r="O55" s="50"/>
-      <c r="P55" s="50"/>
-      <c r="Q55" s="46"/>
-      <c r="R55" s="47"/>
-      <c r="S55" s="46"/>
-      <c r="T55" s="48"/>
-      <c r="U55" s="46"/>
+      <c r="O55" s="27"/>
+      <c r="P55" s="27"/>
+      <c r="Q55" s="23"/>
+      <c r="R55" s="24"/>
+      <c r="S55" s="23"/>
+      <c r="T55" s="25"/>
+      <c r="U55" s="23"/>
     </row>
     <row r="56" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
-      <c r="B56" s="49"/>
-      <c r="C56" s="51"/>
-      <c r="D56" s="42"/>
-      <c r="E56" s="49"/>
-      <c r="F56" s="50"/>
-      <c r="G56" s="43"/>
-      <c r="H56" s="50"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="27"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="27"/>
       <c r="I56" s="4"/>
-      <c r="J56" s="44"/>
+      <c r="J56" s="21"/>
       <c r="K56" s="6"/>
       <c r="L56" s="5"/>
       <c r="M56" s="7"/>
       <c r="N56" s="7"/>
-      <c r="O56" s="50"/>
-      <c r="P56" s="50"/>
-      <c r="Q56" s="46"/>
-      <c r="R56" s="47"/>
-      <c r="S56" s="46"/>
-      <c r="T56" s="48"/>
-      <c r="U56" s="46"/>
+      <c r="O56" s="27"/>
+      <c r="P56" s="27"/>
+      <c r="Q56" s="23"/>
+      <c r="R56" s="24"/>
+      <c r="S56" s="23"/>
+      <c r="T56" s="25"/>
+      <c r="U56" s="23"/>
     </row>
     <row r="57" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
-      <c r="B57" s="49"/>
-      <c r="C57" s="51"/>
-      <c r="D57" s="42"/>
-      <c r="E57" s="49"/>
-      <c r="F57" s="50"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="50"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="27"/>
       <c r="I57" s="4"/>
-      <c r="J57" s="44"/>
+      <c r="J57" s="21"/>
       <c r="K57" s="6"/>
       <c r="L57" s="5"/>
       <c r="M57" s="7"/>
       <c r="N57" s="7"/>
-      <c r="O57" s="50"/>
-      <c r="P57" s="50"/>
-      <c r="Q57" s="46"/>
-      <c r="R57" s="47"/>
-      <c r="S57" s="46"/>
-      <c r="T57" s="48"/>
-      <c r="U57" s="46"/>
+      <c r="O57" s="27"/>
+      <c r="P57" s="27"/>
+      <c r="Q57" s="23"/>
+      <c r="R57" s="24"/>
+      <c r="S57" s="23"/>
+      <c r="T57" s="25"/>
+      <c r="U57" s="23"/>
     </row>
     <row r="58" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
-      <c r="B58" s="49"/>
-      <c r="C58" s="51"/>
-      <c r="D58" s="42"/>
-      <c r="E58" s="49"/>
-      <c r="F58" s="50"/>
-      <c r="G58" s="43"/>
-      <c r="H58" s="50"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="27"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="27"/>
       <c r="I58" s="4"/>
-      <c r="J58" s="44"/>
+      <c r="J58" s="21"/>
       <c r="K58" s="6"/>
       <c r="L58" s="5"/>
       <c r="M58" s="7"/>
       <c r="N58" s="7"/>
-      <c r="O58" s="50"/>
-      <c r="P58" s="50"/>
-      <c r="Q58" s="46"/>
-      <c r="R58" s="47"/>
-      <c r="S58" s="46"/>
-      <c r="T58" s="48"/>
-      <c r="U58" s="46"/>
+      <c r="O58" s="27"/>
+      <c r="P58" s="27"/>
+      <c r="Q58" s="23"/>
+      <c r="R58" s="24"/>
+      <c r="S58" s="23"/>
+      <c r="T58" s="25"/>
+      <c r="U58" s="23"/>
     </row>
     <row r="59" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
-      <c r="B59" s="49"/>
-      <c r="C59" s="51"/>
-      <c r="D59" s="42"/>
-      <c r="E59" s="49"/>
-      <c r="F59" s="50"/>
-      <c r="G59" s="43"/>
-      <c r="H59" s="50"/>
+      <c r="B59" s="26"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="27"/>
       <c r="I59" s="4"/>
-      <c r="J59" s="44"/>
+      <c r="J59" s="21"/>
       <c r="K59" s="6"/>
       <c r="L59" s="5"/>
       <c r="M59" s="7"/>
       <c r="N59" s="7"/>
-      <c r="O59" s="50"/>
-      <c r="P59" s="50"/>
-      <c r="Q59" s="46"/>
-      <c r="R59" s="47"/>
-      <c r="S59" s="46"/>
-      <c r="T59" s="48"/>
-      <c r="U59" s="46"/>
+      <c r="O59" s="27"/>
+      <c r="P59" s="27"/>
+      <c r="Q59" s="23"/>
+      <c r="R59" s="24"/>
+      <c r="S59" s="23"/>
+      <c r="T59" s="25"/>
+      <c r="U59" s="23"/>
     </row>
     <row r="60" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
-      <c r="B60" s="49"/>
-      <c r="C60" s="51"/>
-      <c r="D60" s="42"/>
-      <c r="E60" s="49"/>
-      <c r="F60" s="50"/>
-      <c r="G60" s="43"/>
-      <c r="H60" s="50"/>
+      <c r="B60" s="26"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="27"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="27"/>
       <c r="I60" s="4"/>
-      <c r="J60" s="44"/>
+      <c r="J60" s="21"/>
       <c r="K60" s="6"/>
       <c r="L60" s="5"/>
       <c r="M60" s="7"/>
       <c r="N60" s="7"/>
-      <c r="O60" s="50"/>
-      <c r="P60" s="50"/>
-      <c r="Q60" s="46"/>
-      <c r="R60" s="47"/>
-      <c r="S60" s="46"/>
-      <c r="T60" s="48"/>
-      <c r="U60" s="46"/>
+      <c r="O60" s="27"/>
+      <c r="P60" s="27"/>
+      <c r="Q60" s="23"/>
+      <c r="R60" s="24"/>
+      <c r="S60" s="23"/>
+      <c r="T60" s="25"/>
+      <c r="U60" s="23"/>
     </row>
     <row r="61" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
-      <c r="B61" s="49"/>
-      <c r="C61" s="51"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="49"/>
-      <c r="F61" s="50"/>
-      <c r="G61" s="43"/>
-      <c r="H61" s="50"/>
+      <c r="B61" s="26"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="27"/>
       <c r="I61" s="4"/>
-      <c r="J61" s="44"/>
+      <c r="J61" s="21"/>
       <c r="K61" s="6"/>
       <c r="L61" s="5"/>
       <c r="M61" s="7"/>
       <c r="N61" s="7"/>
-      <c r="O61" s="50"/>
-      <c r="P61" s="50"/>
-      <c r="Q61" s="46"/>
-      <c r="R61" s="47"/>
-      <c r="S61" s="46"/>
-      <c r="T61" s="48"/>
-      <c r="U61" s="46"/>
+      <c r="O61" s="27"/>
+      <c r="P61" s="27"/>
+      <c r="Q61" s="23"/>
+      <c r="R61" s="24"/>
+      <c r="S61" s="23"/>
+      <c r="T61" s="25"/>
+      <c r="U61" s="23"/>
     </row>
     <row r="62" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
-      <c r="B62" s="49"/>
-      <c r="C62" s="51"/>
-      <c r="D62" s="42"/>
-      <c r="E62" s="49"/>
-      <c r="F62" s="50"/>
-      <c r="G62" s="43"/>
-      <c r="H62" s="50"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="27"/>
+      <c r="G62" s="20"/>
+      <c r="H62" s="27"/>
       <c r="I62" s="4"/>
-      <c r="J62" s="44"/>
+      <c r="J62" s="21"/>
       <c r="K62" s="6"/>
       <c r="L62" s="5"/>
       <c r="M62" s="7"/>
       <c r="N62" s="7"/>
-      <c r="O62" s="50"/>
-      <c r="P62" s="50"/>
-      <c r="Q62" s="46"/>
-      <c r="R62" s="47"/>
-      <c r="S62" s="46"/>
-      <c r="T62" s="48"/>
-      <c r="U62" s="46"/>
+      <c r="O62" s="27"/>
+      <c r="P62" s="27"/>
+      <c r="Q62" s="23"/>
+      <c r="R62" s="24"/>
+      <c r="S62" s="23"/>
+      <c r="T62" s="25"/>
+      <c r="U62" s="23"/>
     </row>
     <row r="63" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
-      <c r="B63" s="49"/>
-      <c r="C63" s="51"/>
-      <c r="D63" s="42"/>
-      <c r="E63" s="49"/>
-      <c r="F63" s="50"/>
-      <c r="G63" s="43"/>
-      <c r="H63" s="50"/>
+      <c r="B63" s="26"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="27"/>
+      <c r="G63" s="20"/>
+      <c r="H63" s="27"/>
       <c r="I63" s="4"/>
-      <c r="J63" s="44"/>
+      <c r="J63" s="21"/>
       <c r="K63" s="6"/>
       <c r="L63" s="5"/>
       <c r="M63" s="7"/>
       <c r="N63" s="7"/>
-      <c r="O63" s="50"/>
-      <c r="P63" s="50"/>
-      <c r="Q63" s="46"/>
-      <c r="R63" s="47"/>
-      <c r="S63" s="46"/>
-      <c r="T63" s="48"/>
-      <c r="U63" s="46"/>
+      <c r="O63" s="27"/>
+      <c r="P63" s="27"/>
+      <c r="Q63" s="23"/>
+      <c r="R63" s="24"/>
+      <c r="S63" s="23"/>
+      <c r="T63" s="25"/>
+      <c r="U63" s="23"/>
     </row>
     <row r="64" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
-      <c r="B64" s="49"/>
-      <c r="C64" s="51"/>
-      <c r="D64" s="42"/>
-      <c r="E64" s="49"/>
-      <c r="F64" s="50"/>
-      <c r="G64" s="43"/>
-      <c r="H64" s="50"/>
+      <c r="B64" s="26"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="27"/>
+      <c r="G64" s="20"/>
+      <c r="H64" s="27"/>
       <c r="I64" s="4"/>
-      <c r="J64" s="44"/>
+      <c r="J64" s="21"/>
       <c r="K64" s="6"/>
       <c r="L64" s="5"/>
       <c r="M64" s="7"/>
       <c r="N64" s="7"/>
-      <c r="O64" s="50"/>
-      <c r="P64" s="50"/>
-      <c r="Q64" s="46"/>
-      <c r="R64" s="47"/>
-      <c r="S64" s="46"/>
-      <c r="T64" s="48"/>
-      <c r="U64" s="46"/>
+      <c r="O64" s="27"/>
+      <c r="P64" s="27"/>
+      <c r="Q64" s="23"/>
+      <c r="R64" s="24"/>
+      <c r="S64" s="23"/>
+      <c r="T64" s="25"/>
+      <c r="U64" s="23"/>
     </row>
     <row r="65" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
-      <c r="B65" s="49"/>
-      <c r="C65" s="51"/>
-      <c r="D65" s="42"/>
-      <c r="E65" s="49"/>
-      <c r="F65" s="50"/>
-      <c r="G65" s="43"/>
-      <c r="H65" s="50"/>
+      <c r="B65" s="26"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="27"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="27"/>
       <c r="I65" s="4"/>
-      <c r="J65" s="44"/>
+      <c r="J65" s="21"/>
       <c r="K65" s="6"/>
       <c r="L65" s="5"/>
       <c r="M65" s="7"/>
       <c r="N65" s="7"/>
-      <c r="O65" s="50"/>
-      <c r="P65" s="50"/>
-      <c r="Q65" s="46"/>
-      <c r="R65" s="47"/>
-      <c r="S65" s="46"/>
-      <c r="T65" s="48"/>
-      <c r="U65" s="46"/>
+      <c r="O65" s="27"/>
+      <c r="P65" s="27"/>
+      <c r="Q65" s="23"/>
+      <c r="R65" s="24"/>
+      <c r="S65" s="23"/>
+      <c r="T65" s="25"/>
+      <c r="U65" s="23"/>
     </row>
     <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
-      <c r="B66" s="49"/>
-      <c r="C66" s="51"/>
-      <c r="D66" s="42"/>
-      <c r="E66" s="49"/>
-      <c r="F66" s="50"/>
-      <c r="G66" s="43"/>
-      <c r="H66" s="50"/>
+      <c r="B66" s="26"/>
+      <c r="C66" s="28"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="26"/>
+      <c r="F66" s="27"/>
+      <c r="G66" s="20"/>
+      <c r="H66" s="27"/>
       <c r="I66" s="4"/>
-      <c r="J66" s="44"/>
+      <c r="J66" s="21"/>
       <c r="K66" s="6"/>
       <c r="L66" s="5"/>
       <c r="M66" s="7"/>
       <c r="N66" s="7"/>
-      <c r="O66" s="50"/>
-      <c r="P66" s="50"/>
-      <c r="Q66" s="46"/>
-      <c r="R66" s="47"/>
-      <c r="S66" s="46"/>
-      <c r="T66" s="48"/>
-      <c r="U66" s="46"/>
+      <c r="O66" s="27"/>
+      <c r="P66" s="27"/>
+      <c r="Q66" s="23"/>
+      <c r="R66" s="24"/>
+      <c r="S66" s="23"/>
+      <c r="T66" s="25"/>
+      <c r="U66" s="23"/>
     </row>
     <row r="67" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
-      <c r="B67" s="49"/>
-      <c r="C67" s="51"/>
-      <c r="D67" s="42"/>
-      <c r="E67" s="49"/>
-      <c r="F67" s="50"/>
-      <c r="G67" s="43"/>
-      <c r="H67" s="50"/>
+      <c r="B67" s="26"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="27"/>
+      <c r="G67" s="20"/>
+      <c r="H67" s="27"/>
       <c r="I67" s="4"/>
-      <c r="J67" s="44"/>
+      <c r="J67" s="21"/>
       <c r="K67" s="6"/>
       <c r="L67" s="5"/>
       <c r="M67" s="7"/>
       <c r="N67" s="7"/>
-      <c r="O67" s="50"/>
-      <c r="P67" s="50"/>
-      <c r="Q67" s="46"/>
-      <c r="R67" s="47"/>
-      <c r="S67" s="46"/>
-      <c r="T67" s="48"/>
-      <c r="U67" s="46"/>
+      <c r="O67" s="27"/>
+      <c r="P67" s="27"/>
+      <c r="Q67" s="23"/>
+      <c r="R67" s="24"/>
+      <c r="S67" s="23"/>
+      <c r="T67" s="25"/>
+      <c r="U67" s="23"/>
     </row>
     <row r="68" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
-      <c r="B68" s="49"/>
-      <c r="C68" s="51"/>
-      <c r="D68" s="42"/>
-      <c r="E68" s="49"/>
-      <c r="F68" s="50"/>
-      <c r="G68" s="43"/>
-      <c r="H68" s="50"/>
+      <c r="B68" s="26"/>
+      <c r="C68" s="28"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="27"/>
+      <c r="G68" s="20"/>
+      <c r="H68" s="27"/>
       <c r="I68" s="4"/>
-      <c r="J68" s="44"/>
+      <c r="J68" s="21"/>
       <c r="K68" s="6"/>
       <c r="L68" s="5"/>
       <c r="M68" s="7"/>
       <c r="N68" s="7"/>
-      <c r="O68" s="50"/>
-      <c r="P68" s="50"/>
-      <c r="Q68" s="46"/>
-      <c r="R68" s="47"/>
-      <c r="S68" s="46"/>
-      <c r="T68" s="48"/>
-      <c r="U68" s="46"/>
+      <c r="O68" s="27"/>
+      <c r="P68" s="27"/>
+      <c r="Q68" s="23"/>
+      <c r="R68" s="24"/>
+      <c r="S68" s="23"/>
+      <c r="T68" s="25"/>
+      <c r="U68" s="23"/>
     </row>
     <row r="69" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
-      <c r="B69" s="49"/>
-      <c r="C69" s="51"/>
-      <c r="D69" s="42"/>
-      <c r="E69" s="49"/>
-      <c r="F69" s="50"/>
-      <c r="G69" s="43"/>
-      <c r="H69" s="50"/>
+      <c r="B69" s="26"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="27"/>
+      <c r="G69" s="20"/>
+      <c r="H69" s="27"/>
       <c r="I69" s="4"/>
-      <c r="J69" s="44"/>
+      <c r="J69" s="21"/>
       <c r="K69" s="6"/>
       <c r="L69" s="5"/>
       <c r="M69" s="7"/>
       <c r="N69" s="7"/>
-      <c r="O69" s="50"/>
-      <c r="P69" s="50"/>
-      <c r="Q69" s="46"/>
-      <c r="R69" s="47"/>
-      <c r="S69" s="46"/>
-      <c r="T69" s="48"/>
-      <c r="U69" s="46"/>
+      <c r="O69" s="27"/>
+      <c r="P69" s="27"/>
+      <c r="Q69" s="23"/>
+      <c r="R69" s="24"/>
+      <c r="S69" s="23"/>
+      <c r="T69" s="25"/>
+      <c r="U69" s="23"/>
     </row>
     <row r="70" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
-      <c r="B70" s="49"/>
-      <c r="C70" s="51"/>
-      <c r="D70" s="42"/>
-      <c r="E70" s="49"/>
-      <c r="F70" s="50"/>
-      <c r="G70" s="43"/>
-      <c r="H70" s="50"/>
+      <c r="B70" s="26"/>
+      <c r="C70" s="28"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="26"/>
+      <c r="F70" s="27"/>
+      <c r="G70" s="20"/>
+      <c r="H70" s="27"/>
       <c r="I70" s="4"/>
-      <c r="J70" s="44"/>
+      <c r="J70" s="21"/>
       <c r="K70" s="6"/>
       <c r="L70" s="5"/>
       <c r="M70" s="7"/>
       <c r="N70" s="7"/>
-      <c r="O70" s="50"/>
-      <c r="P70" s="50"/>
-      <c r="Q70" s="46"/>
-      <c r="R70" s="47"/>
-      <c r="S70" s="46"/>
-      <c r="T70" s="48"/>
-      <c r="U70" s="46"/>
+      <c r="O70" s="27"/>
+      <c r="P70" s="27"/>
+      <c r="Q70" s="23"/>
+      <c r="R70" s="24"/>
+      <c r="S70" s="23"/>
+      <c r="T70" s="25"/>
+      <c r="U70" s="23"/>
     </row>
     <row r="71" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
-      <c r="B71" s="49"/>
-      <c r="C71" s="51"/>
-      <c r="D71" s="42"/>
-      <c r="E71" s="49"/>
-      <c r="F71" s="50"/>
-      <c r="G71" s="43"/>
-      <c r="H71" s="50"/>
+      <c r="B71" s="26"/>
+      <c r="C71" s="28"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="27"/>
+      <c r="G71" s="20"/>
+      <c r="H71" s="27"/>
       <c r="I71" s="4"/>
-      <c r="J71" s="44"/>
+      <c r="J71" s="21"/>
       <c r="K71" s="6"/>
       <c r="L71" s="5"/>
       <c r="M71" s="7"/>
       <c r="N71" s="7"/>
-      <c r="O71" s="50"/>
-      <c r="P71" s="50"/>
-      <c r="Q71" s="46"/>
-      <c r="R71" s="47"/>
-      <c r="S71" s="46"/>
-      <c r="T71" s="48"/>
-      <c r="U71" s="46"/>
+      <c r="O71" s="27"/>
+      <c r="P71" s="27"/>
+      <c r="Q71" s="23"/>
+      <c r="R71" s="24"/>
+      <c r="S71" s="23"/>
+      <c r="T71" s="25"/>
+      <c r="U71" s="23"/>
     </row>
     <row r="72" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
-      <c r="B72" s="49"/>
-      <c r="C72" s="51"/>
-      <c r="D72" s="42"/>
-      <c r="E72" s="49"/>
-      <c r="F72" s="50"/>
-      <c r="G72" s="43"/>
-      <c r="H72" s="50"/>
+      <c r="B72" s="26"/>
+      <c r="C72" s="28"/>
+      <c r="D72" s="19"/>
+      <c r="E72" s="26"/>
+      <c r="F72" s="27"/>
+      <c r="G72" s="20"/>
+      <c r="H72" s="27"/>
       <c r="I72" s="4"/>
-      <c r="J72" s="44"/>
+      <c r="J72" s="21"/>
       <c r="K72" s="6"/>
       <c r="L72" s="5"/>
       <c r="M72" s="7"/>
       <c r="N72" s="7"/>
-      <c r="O72" s="50"/>
-      <c r="P72" s="50"/>
-      <c r="Q72" s="46"/>
-      <c r="R72" s="47"/>
-      <c r="S72" s="46"/>
-      <c r="T72" s="48"/>
-      <c r="U72" s="46"/>
+      <c r="O72" s="27"/>
+      <c r="P72" s="27"/>
+      <c r="Q72" s="23"/>
+      <c r="R72" s="24"/>
+      <c r="S72" s="23"/>
+      <c r="T72" s="25"/>
+      <c r="U72" s="23"/>
     </row>
     <row r="73" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
-      <c r="B73" s="49"/>
-      <c r="C73" s="51"/>
-      <c r="D73" s="42"/>
-      <c r="E73" s="49"/>
-      <c r="F73" s="50"/>
-      <c r="G73" s="43"/>
-      <c r="H73" s="50"/>
+      <c r="B73" s="26"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="26"/>
+      <c r="F73" s="27"/>
+      <c r="G73" s="20"/>
+      <c r="H73" s="27"/>
       <c r="I73" s="4"/>
-      <c r="J73" s="44"/>
+      <c r="J73" s="21"/>
       <c r="K73" s="6"/>
       <c r="L73" s="5"/>
       <c r="M73" s="7"/>
       <c r="N73" s="7"/>
-      <c r="O73" s="50"/>
-      <c r="P73" s="50"/>
-      <c r="Q73" s="46"/>
-      <c r="R73" s="47"/>
-      <c r="S73" s="46"/>
-      <c r="T73" s="48"/>
-      <c r="U73" s="46"/>
+      <c r="O73" s="27"/>
+      <c r="P73" s="27"/>
+      <c r="Q73" s="23"/>
+      <c r="R73" s="24"/>
+      <c r="S73" s="23"/>
+      <c r="T73" s="25"/>
+      <c r="U73" s="23"/>
     </row>
     <row r="74" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
-      <c r="B74" s="49"/>
-      <c r="C74" s="51"/>
-      <c r="D74" s="42"/>
-      <c r="E74" s="49"/>
-      <c r="F74" s="50"/>
-      <c r="G74" s="43"/>
-      <c r="H74" s="50"/>
+      <c r="B74" s="26"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="26"/>
+      <c r="F74" s="27"/>
+      <c r="G74" s="20"/>
+      <c r="H74" s="27"/>
       <c r="I74" s="4"/>
-      <c r="J74" s="44"/>
+      <c r="J74" s="21"/>
       <c r="K74" s="6"/>
       <c r="L74" s="5"/>
       <c r="M74" s="7"/>
       <c r="N74" s="7"/>
-      <c r="O74" s="50"/>
-      <c r="P74" s="50"/>
-      <c r="Q74" s="46"/>
-      <c r="R74" s="47"/>
-      <c r="S74" s="46"/>
-      <c r="T74" s="48"/>
-      <c r="U74" s="46"/>
+      <c r="O74" s="27"/>
+      <c r="P74" s="27"/>
+      <c r="Q74" s="23"/>
+      <c r="R74" s="24"/>
+      <c r="S74" s="23"/>
+      <c r="T74" s="25"/>
+      <c r="U74" s="23"/>
     </row>
     <row r="75" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
-      <c r="B75" s="49"/>
-      <c r="C75" s="51"/>
-      <c r="D75" s="42"/>
-      <c r="E75" s="49"/>
-      <c r="F75" s="50"/>
-      <c r="G75" s="43"/>
-      <c r="H75" s="50"/>
+      <c r="B75" s="26"/>
+      <c r="C75" s="28"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="26"/>
+      <c r="F75" s="27"/>
+      <c r="G75" s="20"/>
+      <c r="H75" s="27"/>
       <c r="I75" s="4"/>
-      <c r="J75" s="44"/>
+      <c r="J75" s="21"/>
       <c r="K75" s="6"/>
       <c r="L75" s="5"/>
       <c r="M75" s="7"/>
       <c r="N75" s="7"/>
-      <c r="O75" s="50"/>
-      <c r="P75" s="50"/>
-      <c r="Q75" s="46"/>
-      <c r="R75" s="47"/>
-      <c r="S75" s="46"/>
-      <c r="T75" s="48"/>
-      <c r="U75" s="46"/>
+      <c r="O75" s="27"/>
+      <c r="P75" s="27"/>
+      <c r="Q75" s="23"/>
+      <c r="R75" s="24"/>
+      <c r="S75" s="23"/>
+      <c r="T75" s="25"/>
+      <c r="U75" s="23"/>
     </row>
     <row r="76" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
-      <c r="B76" s="49"/>
-      <c r="C76" s="51"/>
-      <c r="D76" s="42"/>
-      <c r="E76" s="49"/>
-      <c r="F76" s="50"/>
-      <c r="G76" s="43"/>
-      <c r="H76" s="50"/>
+      <c r="B76" s="26"/>
+      <c r="C76" s="28"/>
+      <c r="D76" s="19"/>
+      <c r="E76" s="26"/>
+      <c r="F76" s="27"/>
+      <c r="G76" s="20"/>
+      <c r="H76" s="27"/>
       <c r="I76" s="4"/>
-      <c r="J76" s="44"/>
+      <c r="J76" s="21"/>
       <c r="K76" s="6"/>
       <c r="L76" s="5"/>
       <c r="M76" s="7"/>
       <c r="N76" s="7"/>
-      <c r="O76" s="50"/>
-      <c r="P76" s="50"/>
-      <c r="Q76" s="46"/>
-      <c r="R76" s="47"/>
-      <c r="S76" s="46"/>
-      <c r="T76" s="48"/>
-      <c r="U76" s="46"/>
+      <c r="O76" s="27"/>
+      <c r="P76" s="27"/>
+      <c r="Q76" s="23"/>
+      <c r="R76" s="24"/>
+      <c r="S76" s="23"/>
+      <c r="T76" s="25"/>
+      <c r="U76" s="23"/>
     </row>
     <row r="77" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
-      <c r="B77" s="49"/>
-      <c r="C77" s="51"/>
-      <c r="D77" s="42"/>
-      <c r="E77" s="49"/>
-      <c r="F77" s="50"/>
-      <c r="G77" s="43"/>
-      <c r="H77" s="50"/>
+      <c r="B77" s="26"/>
+      <c r="C77" s="28"/>
+      <c r="D77" s="19"/>
+      <c r="E77" s="26"/>
+      <c r="F77" s="27"/>
+      <c r="G77" s="20"/>
+      <c r="H77" s="27"/>
       <c r="I77" s="4"/>
-      <c r="J77" s="44"/>
+      <c r="J77" s="21"/>
       <c r="K77" s="6"/>
       <c r="L77" s="5"/>
       <c r="M77" s="7"/>
       <c r="N77" s="7"/>
-      <c r="O77" s="50"/>
-      <c r="P77" s="50"/>
-      <c r="Q77" s="46"/>
-      <c r="R77" s="47"/>
-      <c r="S77" s="46"/>
-      <c r="T77" s="48"/>
-      <c r="U77" s="46"/>
+      <c r="O77" s="27"/>
+      <c r="P77" s="27"/>
+      <c r="Q77" s="23"/>
+      <c r="R77" s="24"/>
+      <c r="S77" s="23"/>
+      <c r="T77" s="25"/>
+      <c r="U77" s="23"/>
     </row>
     <row r="78" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
-      <c r="B78" s="49"/>
-      <c r="C78" s="51"/>
-      <c r="D78" s="42"/>
-      <c r="E78" s="49"/>
-      <c r="F78" s="50"/>
-      <c r="G78" s="43"/>
-      <c r="H78" s="50"/>
+      <c r="B78" s="26"/>
+      <c r="C78" s="28"/>
+      <c r="D78" s="19"/>
+      <c r="E78" s="26"/>
+      <c r="F78" s="27"/>
+      <c r="G78" s="20"/>
+      <c r="H78" s="27"/>
       <c r="I78" s="4"/>
-      <c r="J78" s="44"/>
+      <c r="J78" s="21"/>
       <c r="K78" s="6"/>
       <c r="L78" s="5"/>
       <c r="M78" s="7"/>
       <c r="N78" s="7"/>
-      <c r="O78" s="50"/>
-      <c r="P78" s="50"/>
-      <c r="Q78" s="46"/>
-      <c r="R78" s="47"/>
-      <c r="S78" s="46"/>
-      <c r="T78" s="48"/>
-      <c r="U78" s="46"/>
+      <c r="O78" s="27"/>
+      <c r="P78" s="27"/>
+      <c r="Q78" s="23"/>
+      <c r="R78" s="24"/>
+      <c r="S78" s="23"/>
+      <c r="T78" s="25"/>
+      <c r="U78" s="23"/>
     </row>
     <row r="79" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
-      <c r="B79" s="49"/>
-      <c r="C79" s="51"/>
-      <c r="D79" s="42"/>
-      <c r="E79" s="49"/>
-      <c r="F79" s="50"/>
-      <c r="G79" s="43"/>
-      <c r="H79" s="50"/>
+      <c r="B79" s="26"/>
+      <c r="C79" s="28"/>
+      <c r="D79" s="19"/>
+      <c r="E79" s="26"/>
+      <c r="F79" s="27"/>
+      <c r="G79" s="20"/>
+      <c r="H79" s="27"/>
       <c r="I79" s="4"/>
-      <c r="J79" s="44"/>
+      <c r="J79" s="21"/>
       <c r="K79" s="6"/>
       <c r="L79" s="5"/>
       <c r="M79" s="7"/>
       <c r="N79" s="7"/>
-      <c r="O79" s="50"/>
-      <c r="P79" s="50"/>
-      <c r="Q79" s="46"/>
-      <c r="R79" s="47"/>
-      <c r="S79" s="46"/>
-      <c r="T79" s="48"/>
-      <c r="U79" s="46"/>
+      <c r="O79" s="27"/>
+      <c r="P79" s="27"/>
+      <c r="Q79" s="23"/>
+      <c r="R79" s="24"/>
+      <c r="S79" s="23"/>
+      <c r="T79" s="25"/>
+      <c r="U79" s="23"/>
     </row>
     <row r="80" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
-      <c r="B80" s="49"/>
-      <c r="C80" s="51"/>
-      <c r="D80" s="42"/>
-      <c r="E80" s="49"/>
-      <c r="F80" s="50"/>
-      <c r="G80" s="43"/>
-      <c r="H80" s="50"/>
+      <c r="B80" s="26"/>
+      <c r="C80" s="28"/>
+      <c r="D80" s="19"/>
+      <c r="E80" s="26"/>
+      <c r="F80" s="27"/>
+      <c r="G80" s="20"/>
+      <c r="H80" s="27"/>
       <c r="I80" s="4"/>
-      <c r="J80" s="44"/>
+      <c r="J80" s="21"/>
       <c r="K80" s="6"/>
       <c r="L80" s="5"/>
       <c r="M80" s="7"/>
       <c r="N80" s="7"/>
-      <c r="O80" s="50"/>
-      <c r="P80" s="50"/>
-      <c r="Q80" s="46"/>
-      <c r="R80" s="47"/>
-      <c r="S80" s="46"/>
-      <c r="T80" s="48"/>
-      <c r="U80" s="46"/>
+      <c r="O80" s="27"/>
+      <c r="P80" s="27"/>
+      <c r="Q80" s="23"/>
+      <c r="R80" s="24"/>
+      <c r="S80" s="23"/>
+      <c r="T80" s="25"/>
+      <c r="U80" s="23"/>
     </row>
     <row r="81" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
-      <c r="B81" s="49"/>
-      <c r="C81" s="51"/>
-      <c r="D81" s="42"/>
-      <c r="E81" s="49"/>
-      <c r="F81" s="50"/>
-      <c r="G81" s="43"/>
-      <c r="H81" s="50"/>
+      <c r="B81" s="26"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="19"/>
+      <c r="E81" s="26"/>
+      <c r="F81" s="27"/>
+      <c r="G81" s="20"/>
+      <c r="H81" s="27"/>
       <c r="I81" s="4"/>
-      <c r="J81" s="44"/>
+      <c r="J81" s="21"/>
       <c r="K81" s="6"/>
       <c r="L81" s="5"/>
       <c r="M81" s="7"/>
       <c r="N81" s="7"/>
-      <c r="O81" s="50"/>
-      <c r="P81" s="50"/>
-      <c r="Q81" s="46"/>
-      <c r="R81" s="47"/>
-      <c r="S81" s="46"/>
-      <c r="T81" s="48"/>
-      <c r="U81" s="46"/>
+      <c r="O81" s="27"/>
+      <c r="P81" s="27"/>
+      <c r="Q81" s="23"/>
+      <c r="R81" s="24"/>
+      <c r="S81" s="23"/>
+      <c r="T81" s="25"/>
+      <c r="U81" s="23"/>
     </row>
     <row r="82" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
-      <c r="B82" s="49"/>
-      <c r="C82" s="51"/>
-      <c r="D82" s="42"/>
-      <c r="E82" s="49"/>
-      <c r="F82" s="50"/>
-      <c r="G82" s="43"/>
-      <c r="H82" s="50"/>
+      <c r="B82" s="26"/>
+      <c r="C82" s="28"/>
+      <c r="D82" s="19"/>
+      <c r="E82" s="26"/>
+      <c r="F82" s="27"/>
+      <c r="G82" s="20"/>
+      <c r="H82" s="27"/>
       <c r="I82" s="4"/>
-      <c r="J82" s="44"/>
+      <c r="J82" s="21"/>
       <c r="K82" s="6"/>
       <c r="L82" s="5"/>
       <c r="M82" s="7"/>
       <c r="N82" s="7"/>
-      <c r="O82" s="50"/>
-      <c r="P82" s="50"/>
-      <c r="Q82" s="46"/>
-      <c r="R82" s="47"/>
-      <c r="S82" s="46"/>
-      <c r="T82" s="48"/>
-      <c r="U82" s="46"/>
+      <c r="O82" s="27"/>
+      <c r="P82" s="27"/>
+      <c r="Q82" s="23"/>
+      <c r="R82" s="24"/>
+      <c r="S82" s="23"/>
+      <c r="T82" s="25"/>
+      <c r="U82" s="23"/>
     </row>
     <row r="84" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="85" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
@@ -4256,187 +4261,187 @@
     <row r="95" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="96" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="29" t="s">
+      <c r="A97" s="17" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="29" t="s">
+      <c r="A98" s="17" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="29" t="s">
+      <c r="A99" s="17" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="29" t="s">
+      <c r="A100" s="17" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="29" t="s">
+      <c r="A101" s="17" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="29" t="s">
+      <c r="A102" s="17" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="29" t="s">
+      <c r="A103" s="17" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="29" t="s">
+      <c r="A104" s="17" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="29" t="s">
+      <c r="A105" s="17" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="29" t="s">
+      <c r="A106" s="17" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="29" t="s">
+      <c r="A107" s="17" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="29" t="s">
+      <c r="A108" s="17" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="29" t="s">
+      <c r="A109" s="17" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="29" t="s">
+      <c r="A110" s="17" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="29" t="s">
+      <c r="A111" s="17" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="29" t="s">
+      <c r="A112" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="29" t="s">
+      <c r="A113" s="17" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="29" t="s">
+      <c r="A114" s="17" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="29" t="s">
+      <c r="A115" s="17" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="29" t="s">
+      <c r="A116" s="17" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="29" t="s">
+      <c r="A117" s="17" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="29" t="s">
+      <c r="A118" s="17" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="29" t="s">
+      <c r="A119" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="29" t="s">
+      <c r="A120" s="17" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="29" t="s">
+      <c r="A121" s="17" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="29" t="s">
+      <c r="A122" s="17" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="29" t="s">
+      <c r="A123" s="17" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="29" t="s">
+      <c r="A124" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="29" t="s">
+      <c r="A125" s="17" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="29" t="s">
+      <c r="A126" s="17" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="29" t="s">
+      <c r="A127" s="17" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="29" t="s">
+      <c r="A128" s="17" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="129" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="29" t="s">
+      <c r="A129" s="17" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="130" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="29" t="s">
+      <c r="A130" s="17" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="131" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="29" t="s">
+      <c r="A131" s="17" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="132" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="29" t="s">
+      <c r="A132" s="17" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="133" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="29" t="s">
+      <c r="A133" s="17" t="s">
         <v>115</v>
       </c>
     </row>
@@ -4605,12 +4610,6 @@
     <row r="296" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4625,6 +4624,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>